<commit_message>
added transaction management (at last - about 3 days of dicking about there) as well as some new services for the iphone app
</commit_message>
<xml_diff>
--- a/db/courseLoadHelper.xlsx
+++ b/db/courseLoadHelper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16400" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BB-Black" sheetId="4" r:id="rId1"/>
@@ -123,8 +123,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -196,7 +202,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -228,6 +234,9 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -259,6 +268,9 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -590,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -624,6 +636,10 @@
         <f>LOWER(B2)</f>
         <v>black</v>
       </c>
+      <c r="D2" t="str">
+        <f>UPPER(B2)</f>
+        <v>BLACK</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -640,29 +656,33 @@
       <c r="B4" s="2">
         <v>128</v>
       </c>
+      <c r="H4" t="str">
+        <f>"Course "&amp;C2&amp;" = new Course();"</f>
+        <v>Course black = new Course();</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="H5" t="str">
-        <f>"Course "&amp;C2&amp;" = new Course();"</f>
-        <v>Course black = new Course();</v>
+        <f>C2&amp;".setPar("&amp;B3&amp;");"</f>
+        <v>black.setPar(72);</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="H6" t="str">
-        <f>C2&amp;".setPar("&amp;B3&amp;");"</f>
-        <v>black.setPar(72);</v>
+        <f>C2&amp;".setCourseName("""&amp;B1&amp;" "&amp;B2&amp;""");"</f>
+        <v>black.setCourseName("Butter Brook GC Black");</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="H7" t="str">
-        <f>C2&amp;".setCourseName("""&amp;B1&amp;""");"</f>
-        <v>black.setCourseName("Butter Brook GC");</v>
+        <f>C2&amp;".setSlopeIndex("&amp;B4&amp;");"</f>
+        <v>black.setSlopeIndex(128);</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="H8" t="str">
-        <f>C2&amp;".setSlopeIndex("&amp;B4&amp;");"</f>
-        <v>black.setSlopeIndex(128);</v>
+        <f>C2&amp;".setTeeColour(TeeColour."&amp;D2&amp;");"</f>
+        <v>black.setTeeColour(TeeColour.BLACK);</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1031,7 +1051,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:H29"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1064,6 +1084,10 @@
         <f>LOWER(B2)</f>
         <v>blue</v>
       </c>
+      <c r="D2" t="str">
+        <f>UPPER(B2)</f>
+        <v>BLUE</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -1080,29 +1104,33 @@
       <c r="B4" s="2">
         <v>128</v>
       </c>
+      <c r="H4" t="str">
+        <f>"Course "&amp;C2&amp;" = new Course();"</f>
+        <v>Course blue = new Course();</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="H5" t="str">
-        <f>"Course "&amp;C2&amp;" = new Course();"</f>
-        <v>Course blue = new Course();</v>
+        <f>C2&amp;".setPar("&amp;B3&amp;");"</f>
+        <v>blue.setPar(72);</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="H6" t="str">
-        <f>C2&amp;".setPar("&amp;B3&amp;");"</f>
-        <v>blue.setPar(72);</v>
+        <f>C2&amp;".setCourseName("""&amp;B1&amp;" "&amp;B2&amp;""");"</f>
+        <v>blue.setCourseName("Butter Brook GC Blue");</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="H7" t="str">
-        <f>C2&amp;".setCourseName("""&amp;B1&amp;""");"</f>
-        <v>blue.setCourseName("Butter Brook GC");</v>
+        <f>C2&amp;".setSlopeIndex("&amp;B4&amp;");"</f>
+        <v>blue.setSlopeIndex(128);</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="H8" t="str">
-        <f>C2&amp;".setSlopeIndex("&amp;B4&amp;");"</f>
-        <v>blue.setSlopeIndex(128);</v>
+        <f>C2&amp;".setTeeColour(TeeColour."&amp;D2&amp;");"</f>
+        <v>blue.setTeeColour(TeeColour.BLUE);</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1471,7 +1499,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:H29"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1504,6 +1532,10 @@
         <f>LOWER(B2)</f>
         <v>white</v>
       </c>
+      <c r="D2" t="str">
+        <f>UPPER(B2)</f>
+        <v>WHITE</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -1520,29 +1552,33 @@
       <c r="B4" s="2">
         <v>128</v>
       </c>
+      <c r="H4" t="str">
+        <f>"Course "&amp;C2&amp;" = new Course();"</f>
+        <v>Course white = new Course();</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="H5" t="str">
-        <f>"Course "&amp;C2&amp;" = new Course();"</f>
-        <v>Course white = new Course();</v>
+        <f>C2&amp;".setPar("&amp;B3&amp;");"</f>
+        <v>white.setPar(72);</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="H6" t="str">
-        <f>C2&amp;".setPar("&amp;B3&amp;");"</f>
-        <v>white.setPar(72);</v>
+        <f>C2&amp;".setCourseName("""&amp;B1&amp;" "&amp;B2&amp;""");"</f>
+        <v>white.setCourseName("Butter Brook GC White");</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="H7" t="str">
-        <f>C2&amp;".setCourseName("""&amp;B1&amp;""");"</f>
-        <v>white.setCourseName("Butter Brook GC");</v>
+        <f>C2&amp;".setSlopeIndex("&amp;B4&amp;");"</f>
+        <v>white.setSlopeIndex(128);</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="H8" t="str">
-        <f>C2&amp;".setSlopeIndex("&amp;B4&amp;");"</f>
-        <v>white.setSlopeIndex(128);</v>
+        <f>C2&amp;".setTeeColour(TeeColour."&amp;D2&amp;");"</f>
+        <v>white.setTeeColour(TeeColour.WHITE);</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1910,8 +1946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:H29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1944,6 +1980,10 @@
         <f>LOWER(B2)</f>
         <v>red</v>
       </c>
+      <c r="D2" t="str">
+        <f>UPPER(B2)</f>
+        <v>RED</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -1960,29 +2000,33 @@
       <c r="B4" s="2">
         <v>128</v>
       </c>
+      <c r="H4" t="str">
+        <f>"Course "&amp;C2&amp;" = new Course();"</f>
+        <v>Course red = new Course();</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="H5" t="str">
-        <f>"Course "&amp;C2&amp;" = new Course();"</f>
-        <v>Course red = new Course();</v>
+        <f>C2&amp;".setPar("&amp;B3&amp;");"</f>
+        <v>red.setPar(72);</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="H6" t="str">
-        <f>C2&amp;".setPar("&amp;B3&amp;");"</f>
-        <v>red.setPar(72);</v>
+        <f>C2&amp;".setCourseName("""&amp;B1&amp;" "&amp;B2&amp;""");"</f>
+        <v>red.setCourseName("Butter Brook GC Red");</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="H7" t="str">
-        <f>C2&amp;".setCourseName("""&amp;B1&amp;""");"</f>
-        <v>red.setCourseName("Butter Brook GC");</v>
+        <f>C2&amp;".setSlopeIndex("&amp;B4&amp;");"</f>
+        <v>red.setSlopeIndex(128);</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="H8" t="str">
-        <f>C2&amp;".setSlopeIndex("&amp;B4&amp;");"</f>
-        <v>red.setSlopeIndex(128);</v>
+        <f>C2&amp;".setTeeColour(TeeColour."&amp;D2&amp;");"</f>
+        <v>red.setTeeColour(TeeColour.RED);</v>
       </c>
     </row>
     <row r="9" spans="1:8">

</xml_diff>